<commit_message>
General renaming of functions and header for algorithm column names for better consistency. all algorithm functions are now lowercase e.g. rs_bestKeeper -> rs_bestkeeper rs_deltaCt -> rs_deltact
rsdialog and an rs_wizzard has been written supplementing rs_batch-functions with better GUI and more options.

Tests has been updated
</commit_message>
<xml_diff>
--- a/inst/exdata/testref/rs_exceltable.xlsx
+++ b/inst/exdata/testref/rs_exceltable.xlsx
@@ -6,11 +6,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="rfStability" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="rfRank" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="rsStability" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="rsRank" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'rfRank'!$A$1:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'rsRank'!$A$1:$F$6</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -18,19 +18,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t xml:space="preserve">Gene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delta Ct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bestkeeper</t>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta-Ct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BestKeeper</t>
   </si>
   <si>
     <t xml:space="preserve">Normfinder</t>
   </si>
   <si>
-    <t xml:space="preserve">Genorm</t>
+    <t xml:space="preserve">geNorm</t>
   </si>
   <si>
     <t xml:space="preserve">Comprehensive Rank</t>

</xml_diff>